<commit_message>
fix: improve Project Euler 2 presentation
</commit_message>
<xml_diff>
--- a/Project Euler 002.xlsx
+++ b/Project Euler 002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624C79B5-D48F-45F5-AEAD-62C9E09A4B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C4D91B-518C-4799-959D-1857AC030FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2F4E7E5-F8D0-4FB1-955E-13A5EC43899C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Successive Fibonacci numbers</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>&lt;-- answer</t>
+  </si>
+  <si>
+    <t>Project Euler 2: Even Fibonacci Numbers</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23309776-32EB-4532-B969-80178F4379F0}">
-  <dimension ref="B2:E36"/>
+  <dimension ref="B2:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,93 +448,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D2" s="4">
-        <f>SUM(D5:D36)</f>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="4">
+        <f>SUM(D7:D38)</f>
         <v>4613732</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="6" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C5" s="1">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
-        <f>IF(ISEVEN(C5),C5,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" ref="D6:D36" si="0">IF(ISEVEN(C6),C6,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="1">
-        <f>C6</f>
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <f>B7+B6</f>
-        <v>3</v>
-      </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(ISEVEN(C7),C7,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B36" si="1">C7</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C36" si="2">B8+B7</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D8:D38" si="0">IF(ISEVEN(C8),C8,0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>C8</f>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f>B9+B8</f>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" ref="B10:B38" si="1">C9</f>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" ref="C10:C38" si="2">B10+B9</f>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
@@ -541,39 +521,39 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
@@ -583,39 +563,39 @@
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="2"/>
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="2"/>
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="2"/>
-        <v>233</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
@@ -625,39 +605,39 @@
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="2"/>
-        <v>377</v>
+        <v>144</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <f t="shared" si="1"/>
-        <v>377</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="2"/>
-        <v>610</v>
+        <v>233</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>610</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <f t="shared" si="1"/>
-        <v>610</v>
+        <v>233</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="2"/>
-        <v>987</v>
+        <v>377</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
@@ -667,39 +647,39 @@
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <f t="shared" si="1"/>
-        <v>987</v>
+        <v>377</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="2"/>
-        <v>1597</v>
+        <v>610</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>610</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <f t="shared" si="1"/>
-        <v>1597</v>
+        <v>610</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="2"/>
-        <v>2584</v>
+        <v>987</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>2584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <f t="shared" si="1"/>
-        <v>2584</v>
+        <v>987</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="2"/>
-        <v>4181</v>
+        <v>1597</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
@@ -709,39 +689,39 @@
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <f t="shared" si="1"/>
-        <v>4181</v>
+        <v>1597</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="2"/>
-        <v>6765</v>
+        <v>2584</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
         <f t="shared" si="1"/>
-        <v>6765</v>
+        <v>2584</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="2"/>
-        <v>10946</v>
+        <v>4181</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>10946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
         <f t="shared" si="1"/>
-        <v>10946</v>
+        <v>4181</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="2"/>
-        <v>17711</v>
+        <v>6765</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
@@ -751,39 +731,39 @@
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <f t="shared" si="1"/>
-        <v>17711</v>
+        <v>6765</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="2"/>
-        <v>28657</v>
+        <v>10946</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10946</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
         <f t="shared" si="1"/>
-        <v>28657</v>
+        <v>10946</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="2"/>
-        <v>46368</v>
+        <v>17711</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>46368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
         <f t="shared" si="1"/>
-        <v>46368</v>
+        <v>17711</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="2"/>
-        <v>75025</v>
+        <v>28657</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
@@ -793,39 +773,39 @@
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <f t="shared" si="1"/>
-        <v>75025</v>
+        <v>28657</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="2"/>
-        <v>121393</v>
+        <v>46368</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46368</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <f t="shared" si="1"/>
-        <v>121393</v>
+        <v>46368</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="2"/>
-        <v>196418</v>
+        <v>75025</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>196418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <f t="shared" si="1"/>
-        <v>196418</v>
+        <v>75025</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="2"/>
-        <v>317811</v>
+        <v>121393</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
@@ -835,39 +815,39 @@
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <f t="shared" si="1"/>
-        <v>317811</v>
+        <v>121393</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="2"/>
-        <v>514229</v>
+        <v>196418</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>196418</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <f t="shared" si="1"/>
-        <v>514229</v>
+        <v>196418</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="2"/>
-        <v>832040</v>
+        <v>317811</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>832040</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="1">
         <f t="shared" si="1"/>
-        <v>832040</v>
+        <v>317811</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="2"/>
-        <v>1346269</v>
+        <v>514229</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
@@ -877,27 +857,55 @@
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="1">
         <f t="shared" si="1"/>
-        <v>1346269</v>
+        <v>514229</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="2"/>
-        <v>2178309</v>
+        <v>832040</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>832040</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="1">
         <f t="shared" si="1"/>
+        <v>832040</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="2"/>
+        <v>1346269</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="1">
+        <f t="shared" si="1"/>
+        <v>1346269</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="2"/>
         <v>2178309</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="1">
+        <f t="shared" si="1"/>
+        <v>2178309</v>
+      </c>
+      <c r="C38" s="1">
         <f t="shared" si="2"/>
         <v>3524578</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D38" s="1">
         <f t="shared" si="0"/>
         <v>3524578</v>
       </c>

</xml_diff>

<commit_message>
fix: improve Project Euler 2
</commit_message>
<xml_diff>
--- a/Project Euler 002.xlsx
+++ b/Project Euler 002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C4D91B-518C-4799-959D-1857AC030FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10673325-6BD6-4027-B70F-94A6B22270A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2F4E7E5-F8D0-4FB1-955E-13A5EC43899C}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>&lt;-- answer</t>
   </si>
   <si>
-    <t>Project Euler 2: Even Fibonacci Numbers</t>
+    <t>Projec Euler 2: Even Fibonacci numbers</t>
   </si>
 </sst>
 </file>
@@ -74,15 +74,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,18 +96,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,481 +458,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23309776-32EB-4532-B969-80178F4379F0}">
-  <dimension ref="B2:E38"/>
+  <dimension ref="B2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="10.90625" style="1"/>
+    <col min="2" max="3" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="D4" s="4">
-        <f>SUM(D7:D38)</f>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
+        <f>SUM(C8:C39)</f>
         <v>4613732</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
+    <row r="6" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C7" s="1">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
-        <f>IF(ISEVEN(C7),C7,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
+      <c r="C7" s="4">
+        <f>IF(ISEVEN(B7),B7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
+        <f>IF(ISEVEN(B8),B8,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <f>B7+B8</f>
         <v>2</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" ref="D8:D38" si="0">IF(ISEVEN(C8),C8,0)</f>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:C39" si="0">IF(ISEVEN(B9),B9,0)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="1">
-        <f>C8</f>
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <f>B9+B8</f>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <f t="shared" ref="B10:B39" si="1">B8+B9</f>
         <v>3</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="1">
-        <f t="shared" ref="B10:B38" si="1">C9</f>
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" ref="C10:C38" si="2">B10+B9</f>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="2"/>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="2"/>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="2"/>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="2"/>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="D14" s="1">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="1">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="2"/>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="1">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="C16" s="1">
-        <f t="shared" si="2"/>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="1">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="2"/>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
-      <c r="D17" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="1">
-        <f t="shared" si="1"/>
-        <v>144</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="2"/>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <f t="shared" si="1"/>
         <v>233</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
-        <f t="shared" si="1"/>
-        <v>233</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="2"/>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <f t="shared" si="1"/>
         <v>377</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
-        <f t="shared" si="1"/>
-        <v>377</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="2"/>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <f t="shared" si="1"/>
         <v>610</v>
       </c>
-      <c r="D20" s="1">
+      <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>610</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="1">
-        <f t="shared" si="1"/>
-        <v>610</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" si="2"/>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <f t="shared" si="1"/>
         <v>987</v>
       </c>
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="1">
-        <f t="shared" si="1"/>
-        <v>987</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="2"/>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <f t="shared" si="1"/>
         <v>1597</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="1">
-        <f t="shared" si="1"/>
-        <v>1597</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="2"/>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <f t="shared" si="1"/>
         <v>2584</v>
       </c>
-      <c r="D23" s="1">
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>2584</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="1">
-        <f t="shared" si="1"/>
-        <v>2584</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="2"/>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <f t="shared" si="1"/>
         <v>4181</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="1">
-        <f t="shared" si="1"/>
-        <v>4181</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="2"/>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <f t="shared" si="1"/>
         <v>6765</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="1">
-        <f t="shared" si="1"/>
-        <v>6765</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="2"/>
+      <c r="C26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <f t="shared" si="1"/>
         <v>10946</v>
       </c>
-      <c r="D26" s="1">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>10946</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="1">
-        <f t="shared" si="1"/>
-        <v>10946</v>
-      </c>
-      <c r="C27" s="1">
-        <f t="shared" si="2"/>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <f t="shared" si="1"/>
         <v>17711</v>
       </c>
-      <c r="D27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="1">
-        <f t="shared" si="1"/>
-        <v>17711</v>
-      </c>
-      <c r="C28" s="1">
-        <f t="shared" si="2"/>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <f t="shared" si="1"/>
         <v>28657</v>
       </c>
-      <c r="D28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="1">
-        <f t="shared" si="1"/>
-        <v>28657</v>
-      </c>
-      <c r="C29" s="1">
-        <f t="shared" si="2"/>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <f t="shared" si="1"/>
         <v>46368</v>
       </c>
-      <c r="D29" s="1">
+      <c r="C30" s="4">
         <f t="shared" si="0"/>
         <v>46368</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="1">
-        <f t="shared" si="1"/>
-        <v>46368</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="2"/>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <f t="shared" si="1"/>
         <v>75025</v>
       </c>
-      <c r="D30" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="1">
-        <f t="shared" si="1"/>
-        <v>75025</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="2"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <f t="shared" si="1"/>
         <v>121393</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="1">
-        <f t="shared" si="1"/>
-        <v>121393</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="2"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <f t="shared" si="1"/>
         <v>196418</v>
       </c>
-      <c r="D32" s="1">
+      <c r="C33" s="4">
         <f t="shared" si="0"/>
         <v>196418</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="1">
-        <f t="shared" si="1"/>
-        <v>196418</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="2"/>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
+        <f t="shared" si="1"/>
         <v>317811</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="1">
-        <f t="shared" si="1"/>
-        <v>317811</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" si="2"/>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="4">
+        <f t="shared" si="1"/>
         <v>514229</v>
       </c>
-      <c r="D34" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="1">
-        <f t="shared" si="1"/>
-        <v>514229</v>
-      </c>
-      <c r="C35" s="1">
-        <f t="shared" si="2"/>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" s="4">
+        <f t="shared" si="1"/>
         <v>832040</v>
       </c>
-      <c r="D35" s="1">
+      <c r="C36" s="4">
         <f t="shared" si="0"/>
         <v>832040</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="1">
-        <f t="shared" si="1"/>
-        <v>832040</v>
-      </c>
-      <c r="C36" s="1">
-        <f t="shared" si="2"/>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <f t="shared" si="1"/>
         <v>1346269</v>
       </c>
-      <c r="D36" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="1">
-        <f t="shared" si="1"/>
-        <v>1346269</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="2"/>
+      <c r="C37" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="4">
+        <f t="shared" si="1"/>
         <v>2178309</v>
       </c>
-      <c r="D37" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="1">
-        <f t="shared" si="1"/>
-        <v>2178309</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="2"/>
+      <c r="C38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" s="4">
+        <f t="shared" si="1"/>
         <v>3524578</v>
       </c>
-      <c r="D38" s="1">
+      <c r="C39" s="4">
         <f t="shared" si="0"/>
         <v>3524578</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: improve Project Euler 2 and add another method
</commit_message>
<xml_diff>
--- a/Project Euler 002.xlsx
+++ b/Project Euler 002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287BD11F-5631-4DD7-8DF1-0C166F46211D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD5FB05-4863-4C7C-8B80-D80FA236F4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2F4E7E5-F8D0-4FB1-955E-13A5EC43899C}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Successive Fibonacci numbers</t>
   </si>
@@ -75,9 +75,6 @@
     <t>1) As an one-liner using array formulas</t>
   </si>
   <si>
-    <t>2) Using spreadsheets capabilities</t>
-  </si>
-  <si>
     <t>&lt;-- seed</t>
   </si>
   <si>
@@ -85,6 +82,21 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?app=desktop&amp;v=boEyITKWeXM</t>
+  </si>
+  <si>
+    <t>3) Using spreadsheets capabilities</t>
+  </si>
+  <si>
+    <t>https://techcommunity.microsoft.com/t5/excel/hrecurse-instead-of-makearray-recursing-lambda/m-p/3562417</t>
+  </si>
+  <si>
+    <t>Inspiration for use of VSTACK:</t>
+  </si>
+  <si>
+    <t>Note: use optimized, since calculate n-th Fibonacci number for n=1…m</t>
+  </si>
+  <si>
+    <t>2) As an one-liner using array formulas, other solution</t>
   </si>
 </sst>
 </file>
@@ -94,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,17 +123,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="4"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,9 +201,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -186,9 +214,11 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23309776-32EB-4532-B969-80178F4379F0}">
-  <dimension ref="B2:D49"/>
+  <dimension ref="B2:F59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,253 +566,222 @@
     <col min="2" max="3" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:6" ht="16" x14ac:dyDescent="0.4">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="9">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="8">
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C7" s="3" cm="1">
         <f t="array" ref="C7">_xlfn.LET(
-_xlpm.SEED, C6,
-_xlpm.FOUR_MILLIONS, 4000000,
-_xlpm.FIB, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.N=1, 0, INDEX( _xlfn.REDUCE({0;1}, _xlfn.SEQUENCE(_xlpm.N-1), _xlfn.LAMBDA(_xlpm.x,_xlpm.y, IF({1;0}, INDEX(_xlpm.x,2), SUM(_xlpm.x)))), 2 ))),
-IF(_xlpm.FIB(_xlpm.SEED) &lt; _xlpm.FOUR_MILLIONS, "Seed too low",
-_xlfn.LET(
-_xlpm.SEQUENCE_OF_FIB, _xlfn.MAP(_xlfn.SEQUENCE(_xlpm.SEED), _xlpm.FIB),
-_xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS, _xlfn.LAMBDA(_xlpm.N, IF(AND(ISEVEN(_xlpm.N),_xlpm.N&lt;_xlpm.FOUR_MILLIONS), _xlpm.N, 0)),
-SUM(_xlfn.MAP(_xlpm.SEQUENCE_OF_FIB, _xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS)))))</f>
+_xlpm.seed, C6,
+_xlpm.four_millions, 4000000,
+_xlpm.NTH_FIBONACCI_NUMBER, _xlfn.LAMBDA(_xlpm.n, IF(_xlpm.n=1, 0, INDEX( _xlfn.REDUCE({0;1}, _xlfn.SEQUENCE(_xlpm.n-1), _xlfn.LAMBDA(_xlpm.x,_xlpm.y, IF({1;0}, INDEX(_xlpm.x,2), SUM(_xlpm.x)))), 2 ))),
+_xlpm.sequence_of_fib, _xlfn.MAP(_xlfn.SEQUENCE(_xlpm.seed), _xlpm.NTH_FIBONACCI_NUMBER),
+_xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS, _xlfn.LAMBDA(_xlpm.n, IF(AND(ISEVEN(_xlpm.n),_xlpm.n&lt;_xlpm.four_millions), _xlpm.n, 0)),
+IF(_xlpm.NTH_FIBONACCI_NUMBER(_xlpm.seed) &lt; _xlpm.four_millions, "Seed too low",SUM(_xlfn.MAP(_xlpm.sequence_of_fib, _xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS))))</f>
         <v>4613732</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C9" s="11" t="s">
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C10" s="10" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="9"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.4">
+      <c r="B14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="9"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="8">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="3" cm="1">
+        <f t="array" ref="C17">_xlfn.LET(
+_xlpm.seed,C16,
+_xlpm.four_millions,4000000,
+_xlpm.MAKE_SEQUENCE_OF_FIB,_xlfn.LAMBDA(_xlpm.M,_xlfn.REDUCE(0,
+_xlfn.SEQUENCE(_xlpm.M),
+_xlfn.LAMBDA(_xlpm.current_array,_xlpm.n,IF(_xlpm.n=0,0,IF(_xlpm.n=1,_xlfn.VSTACK(0,1),
+_xlfn.LET(_xlpm.new_fibo,_xlfn.HSTACK(INDEX(_xlpm.current_array,_xlpm.n,1)+INDEX(_xlpm.current_array,_xlpm.n-1,1)),_xlfn.VSTACK(_xlpm.current_array,_xlpm.new_fibo))))))),
+_xlpm.sequence_of_fib,_xlpm.MAKE_SEQUENCE_OF_FIB(_xlpm.seed),
+_xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS,_xlfn.LAMBDA(_xlpm.n,IF(AND(ISEVEN(_xlpm.n),_xlpm.n&lt;_xlpm.four_millions),_xlpm.n,0)),
+_xlpm.last_element, INDEX(_xlpm.sequence_of_fib,_xlpm.seed,1),
+IF(_xlpm.last_element&lt;=_xlpm.four_millions, "Seed too low", SUM(_xlfn.MAP(_xlpm.sequence_of_fib,_xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS))))</f>
+        <v>4613732</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="9"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="3">
+        <f>SUM(C28:C59)</f>
+        <v>4613732</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
+        <f>IF(ISEVEN(B27),B27,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4">
+        <f>IF(ISEVEN(B28),B28,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <f>B27+B28</f>
+        <v>2</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:C59" si="0">IF(ISEVEN(B29),B29,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B59" si="1">B28+B29</f>
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C14" s="3">
-        <f>SUM(C18:C49)</f>
-        <v>4613732</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <f>IF(ISEVEN(B17),B17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <f>IF(ISEVEN(B18),B18,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="4">
-        <f>B17+B18</f>
-        <v>2</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" ref="C19:C49" si="0">IF(ISEVEN(B19),B19,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="4">
-        <f t="shared" ref="B20:B49" si="1">B18+B19</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="4">
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C32" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="C25" s="4">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="C26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="C27" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="4">
-        <f t="shared" si="1"/>
-        <v>144</v>
-      </c>
-      <c r="C28" s="4">
-        <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
-        <f t="shared" si="1"/>
-        <v>233</v>
-      </c>
-      <c r="C29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="4">
-        <f t="shared" si="1"/>
-        <v>377</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>610</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="0"/>
-        <v>610</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>987</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <f t="shared" si="1"/>
-        <v>1597</v>
+        <v>13</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="0"/>
@@ -792,27 +791,27 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <f t="shared" si="1"/>
-        <v>2584</v>
+        <v>21</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="0"/>
-        <v>2584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <f t="shared" si="1"/>
-        <v>4181</v>
+        <v>34</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <f t="shared" si="1"/>
-        <v>6765</v>
+        <v>55</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="0"/>
@@ -822,27 +821,27 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <f t="shared" si="1"/>
-        <v>10946</v>
+        <v>89</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="0"/>
-        <v>10946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
         <f t="shared" si="1"/>
-        <v>17711</v>
+        <v>144</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
         <f t="shared" si="1"/>
-        <v>28657</v>
+        <v>233</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
@@ -852,27 +851,27 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="4">
         <f t="shared" si="1"/>
-        <v>46368</v>
+        <v>377</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="0"/>
-        <v>46368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
         <f t="shared" si="1"/>
-        <v>75025</v>
+        <v>610</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>610</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="4">
         <f t="shared" si="1"/>
-        <v>121393</v>
+        <v>987</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="0"/>
@@ -882,27 +881,27 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
         <f t="shared" si="1"/>
-        <v>196418</v>
+        <v>1597</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="0"/>
-        <v>196418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
         <f t="shared" si="1"/>
-        <v>317811</v>
+        <v>2584</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
         <f t="shared" si="1"/>
-        <v>514229</v>
+        <v>4181</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="0"/>
@@ -912,27 +911,27 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="4">
         <f t="shared" si="1"/>
-        <v>832040</v>
+        <v>6765</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="0"/>
-        <v>832040</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
         <f t="shared" si="1"/>
-        <v>1346269</v>
+        <v>10946</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10946</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="4">
         <f t="shared" si="1"/>
-        <v>2178309</v>
+        <v>17711</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="0"/>
@@ -942,18 +941,119 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="4">
         <f t="shared" si="1"/>
+        <v>28657</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" s="4">
+        <f t="shared" si="1"/>
+        <v>46368</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="0"/>
+        <v>46368</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" s="4">
+        <f t="shared" si="1"/>
+        <v>75025</v>
+      </c>
+      <c r="C51" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" s="4">
+        <f t="shared" si="1"/>
+        <v>121393</v>
+      </c>
+      <c r="C52" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" s="4">
+        <f t="shared" si="1"/>
+        <v>196418</v>
+      </c>
+      <c r="C53" s="4">
+        <f t="shared" si="0"/>
+        <v>196418</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" s="4">
+        <f t="shared" si="1"/>
+        <v>317811</v>
+      </c>
+      <c r="C54" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" s="4">
+        <f t="shared" si="1"/>
+        <v>514229</v>
+      </c>
+      <c r="C55" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="4">
+        <f t="shared" si="1"/>
+        <v>832040</v>
+      </c>
+      <c r="C56" s="4">
+        <f t="shared" si="0"/>
+        <v>832040</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" s="4">
+        <f t="shared" si="1"/>
+        <v>1346269</v>
+      </c>
+      <c r="C57" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" s="4">
+        <f t="shared" si="1"/>
+        <v>2178309</v>
+      </c>
+      <c r="C58" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" s="4">
+        <f t="shared" si="1"/>
         <v>3524578</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C59" s="4">
         <f t="shared" si="0"/>
         <v>3524578</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{5702CE18-E124-4AA4-8971-8B28B08A8462}"/>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{5702CE18-E124-4AA4-8971-8B28B08A8462}"/>
+    <hyperlink ref="C20" r:id="rId2" xr:uid="{9FC34E98-EE69-4E7E-BE39-D47C86827131}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: implement minor improvements on Excel files
</commit_message>
<xml_diff>
--- a/Project Euler 002.xlsx
+++ b/Project Euler 002.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD5FB05-4863-4C7C-8B80-D80FA236F4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E305553-3903-4E0D-B44F-AF7D03D8AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2F4E7E5-F8D0-4FB1-955E-13A5EC43899C}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Successive Fibonacci numbers</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>2) As an one-liner using array formulas, other solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each new term in the Fibonacci sequence is generated by adding the previous two terms. </t>
+  </si>
+  <si>
+    <t>By starting with 1 and 2, the first 10 terms will be: 1,2, 3, 5, 8, 13, 21, 34, 55, 89, …</t>
+  </si>
+  <si>
+    <t>By considering the terms in the Fibonacci sequence whose values do not exceed four million, find the sum of the even-valued terms.</t>
   </si>
 </sst>
 </file>
@@ -106,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +159,13 @@
       <b/>
       <sz val="12"/>
       <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -219,10 +235,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -239,7 +256,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -555,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23309776-32EB-4532-B969-80178F4379F0}">
-  <dimension ref="B2:F59"/>
+  <dimension ref="B2:F63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="10.90625" style="1"/>
   </cols>
@@ -571,29 +588,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="2:6" ht="16" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="s">
+    <row r="3" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="2:6" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" ht="16" x14ac:dyDescent="0.4">
+      <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="8">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="8">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="3" cm="1">
-        <f t="array" ref="C7">_xlfn.LET(
-_xlpm.seed, C6,
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="3" cm="1">
+        <f t="array" ref="C11">_xlfn.LET(
+_xlpm.seed, C10,
 _xlpm.four_millions, 4000000,
 _xlpm.NTH_FIBONACCI_NUMBER, _xlfn.LAMBDA(_xlpm.n, IF(_xlpm.n=1, 0, INDEX( _xlfn.REDUCE({0;1}, _xlfn.SEQUENCE(_xlpm.n-1), _xlfn.LAMBDA(_xlpm.x,_xlpm.y, IF({1;0}, INDEX(_xlpm.x,2), SUM(_xlpm.x)))), 2 ))),
 _xlpm.sequence_of_fib, _xlfn.MAP(_xlfn.SEQUENCE(_xlpm.seed), _xlpm.NTH_FIBONACCI_NUMBER),
@@ -601,65 +639,65 @@
 IF(_xlpm.NTH_FIBONACCI_NUMBER(_xlpm.seed) &lt; _xlpm.four_millions, "Seed too low",SUM(_xlfn.MAP(_xlpm.sequence_of_fib, _xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS))))</f>
         <v>4613732</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="13" t="s">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C12" s="9" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="9"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.4">
-      <c r="B14" s="12" t="s">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="9"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B18" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C15" s="9"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C16" s="8">
+      <c r="C18" s="9"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="9"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="8">
         <v>35</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="3" cm="1">
-        <f t="array" ref="C17">_xlfn.LET(
-_xlpm.seed,C16,
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="3" cm="1">
+        <f t="array" ref="C21">_xlfn.LET(
+_xlpm.seed,C20,
 _xlpm.four_millions,4000000,
 _xlpm.MAKE_SEQUENCE_OF_FIB,_xlfn.LAMBDA(_xlpm.M,_xlfn.REDUCE(0,
 _xlfn.SEQUENCE(_xlpm.M),
@@ -671,127 +709,87 @@
 IF(_xlpm.last_element&lt;=_xlpm.four_millions, "Seed too low", SUM(_xlfn.MAP(_xlpm.sequence_of_fib,_xlpm.FILTER_EVEN_AND_BELOW_4_MILLIONS))))</f>
         <v>4613732</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="9"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="1" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="9"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="9" t="s">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="2:5" ht="16" x14ac:dyDescent="0.4">
-      <c r="B22" s="12" t="s">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="2:5" ht="16" x14ac:dyDescent="0.4">
+      <c r="B26" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="3">
-        <f>SUM(C28:C59)</f>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C28" s="3">
+        <f>SUM(C32:C63)</f>
         <v>4613732</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5" t="s">
+    <row r="30" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <f>IF(ISEVEN(B27),B27,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <f>IF(ISEVEN(B28),B28,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
-        <f>B27+B28</f>
-        <v>2</v>
-      </c>
-      <c r="C29" s="4">
-        <f t="shared" ref="C29:C59" si="0">IF(ISEVEN(B29),B29,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="4">
-        <f t="shared" ref="B30:B59" si="1">B28+B29</f>
-        <v>3</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" si="0"/>
+        <f>IF(ISEVEN(B31),B31,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>IF(ISEVEN(B32),B32,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f>B31+B32</f>
+        <v>2</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="C33:C63" si="0">IF(ISEVEN(B33),B33,0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" ref="B34:B63" si="1">B32+B33</f>
+        <v>3</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="0"/>
@@ -801,27 +799,27 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="0"/>
@@ -831,27 +829,27 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>34</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40" s="4">
         <f t="shared" si="1"/>
-        <v>377</v>
+        <v>55</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="0"/>
@@ -861,27 +859,27 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
         <f t="shared" si="1"/>
-        <v>610</v>
+        <v>89</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="0"/>
-        <v>610</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="4">
         <f t="shared" si="1"/>
-        <v>987</v>
+        <v>144</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
         <f t="shared" si="1"/>
-        <v>1597</v>
+        <v>233</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="0"/>
@@ -891,27 +889,27 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="4">
         <f t="shared" si="1"/>
-        <v>2584</v>
+        <v>377</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="0"/>
-        <v>2584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
         <f t="shared" si="1"/>
-        <v>4181</v>
+        <v>610</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>610</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="4">
         <f t="shared" si="1"/>
-        <v>6765</v>
+        <v>987</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="0"/>
@@ -921,27 +919,27 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
         <f t="shared" si="1"/>
-        <v>10946</v>
+        <v>1597</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="0"/>
-        <v>10946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48" s="4">
         <f t="shared" si="1"/>
-        <v>17711</v>
+        <v>2584</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="4">
         <f t="shared" si="1"/>
-        <v>28657</v>
+        <v>4181</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="0"/>
@@ -951,27 +949,27 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50" s="4">
         <f t="shared" si="1"/>
-        <v>46368</v>
+        <v>6765</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="0"/>
-        <v>46368</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="4">
         <f t="shared" si="1"/>
-        <v>75025</v>
+        <v>10946</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10946</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="4">
         <f t="shared" si="1"/>
-        <v>121393</v>
+        <v>17711</v>
       </c>
       <c r="C52" s="4">
         <f t="shared" si="0"/>
@@ -981,27 +979,27 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="4">
         <f t="shared" si="1"/>
-        <v>196418</v>
+        <v>28657</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="0"/>
-        <v>196418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="4">
         <f t="shared" si="1"/>
-        <v>317811</v>
+        <v>46368</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46368</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="4">
         <f t="shared" si="1"/>
-        <v>514229</v>
+        <v>75025</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="0"/>
@@ -1011,27 +1009,27 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56" s="4">
         <f t="shared" si="1"/>
-        <v>832040</v>
+        <v>121393</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="0"/>
-        <v>832040</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="4">
         <f t="shared" si="1"/>
-        <v>1346269</v>
+        <v>196418</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>196418</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="4">
         <f t="shared" si="1"/>
-        <v>2178309</v>
+        <v>317811</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="0"/>
@@ -1041,17 +1039,57 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="4">
         <f t="shared" si="1"/>
+        <v>514229</v>
+      </c>
+      <c r="C59" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" s="4">
+        <f t="shared" si="1"/>
+        <v>832040</v>
+      </c>
+      <c r="C60" s="4">
+        <f t="shared" si="0"/>
+        <v>832040</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" s="4">
+        <f t="shared" si="1"/>
+        <v>1346269</v>
+      </c>
+      <c r="C61" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" s="4">
+        <f t="shared" si="1"/>
+        <v>2178309</v>
+      </c>
+      <c r="C62" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" s="4">
+        <f t="shared" si="1"/>
         <v>3524578</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C63" s="4">
         <f t="shared" si="0"/>
         <v>3524578</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{5702CE18-E124-4AA4-8971-8B28B08A8462}"/>
-    <hyperlink ref="C20" r:id="rId2" xr:uid="{9FC34E98-EE69-4E7E-BE39-D47C86827131}"/>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{5702CE18-E124-4AA4-8971-8B28B08A8462}"/>
+    <hyperlink ref="C24" r:id="rId2" xr:uid="{9FC34E98-EE69-4E7E-BE39-D47C86827131}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
feat: improve solution to Project Euler 8
</commit_message>
<xml_diff>
--- a/Project Euler 002.xlsx
+++ b/Project Euler 002.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E305553-3903-4E0D-B44F-AF7D03D8AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A814A4-78E6-41DE-ADC1-977A9A481C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D2F4E7E5-F8D0-4FB1-955E-13A5EC43899C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -239,7 +239,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -574,11 +574,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23309776-32EB-4532-B969-80178F4379F0}">
   <dimension ref="B2:F63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="10.90625" style="1"/>
   </cols>

</xml_diff>